<commit_message>
Update display for many datasets
</commit_message>
<xml_diff>
--- a/ResultData.xlsx
+++ b/ResultData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="12540" windowWidth="21860" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,28 +210,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -514,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -526,57 +535,57 @@
     <col min="30" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="5" t="s">
+    <row r="2" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="5" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="5" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5" t="s">
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="5" t="s">
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="5" t="s">
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="7"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="16"/>
     </row>
-    <row r="3" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -588,7 +597,7 @@
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -597,10 +606,10 @@
       <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -609,10 +618,10 @@
       <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="P3" s="3" t="s">
@@ -621,10 +630,10 @@
       <c r="Q3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="3" t="s">
@@ -633,10 +642,10 @@
       <c r="U3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="V3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="X3" s="3" t="s">
@@ -645,18 +654,18 @@
       <c r="Y3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="Z3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>0.75</v>
       </c>
       <c r="D4" s="3">
@@ -668,7 +677,7 @@
       <c r="F4" s="3">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>0.72</v>
       </c>
       <c r="H4" s="3">
@@ -677,10 +686,10 @@
       <c r="I4" s="3">
         <v>0.74</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>6.2E-2</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="7">
         <v>0.7</v>
       </c>
       <c r="L4" s="3">
@@ -689,10 +698,10 @@
       <c r="M4" s="3">
         <v>0.78</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="8">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>0.75</v>
       </c>
       <c r="P4" s="3">
@@ -701,10 +710,10 @@
       <c r="Q4" s="3">
         <v>0.81</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="8">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="S4" s="8">
+      <c r="S4" s="7">
         <v>0.69</v>
       </c>
       <c r="T4" s="3">
@@ -713,10 +722,10 @@
       <c r="U4" s="3">
         <v>0.71</v>
       </c>
-      <c r="V4" s="9">
+      <c r="V4" s="8">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="W4" s="8">
+      <c r="W4" s="7">
         <v>0.65</v>
       </c>
       <c r="X4" s="3">
@@ -725,18 +734,18 @@
       <c r="Y4" s="3">
         <v>0.61</v>
       </c>
-      <c r="Z4" s="9">
+      <c r="Z4" s="8">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>0.8</v>
       </c>
       <c r="D5" s="3">
@@ -748,7 +757,7 @@
       <c r="F5" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>0.76</v>
       </c>
       <c r="H5" s="3">
@@ -757,10 +766,10 @@
       <c r="I5" s="3">
         <v>0.77</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <v>0.75</v>
       </c>
       <c r="L5" s="3">
@@ -769,10 +778,10 @@
       <c r="M5" s="3">
         <v>0.81</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="7">
         <v>0.79</v>
       </c>
       <c r="P5" s="3">
@@ -781,10 +790,10 @@
       <c r="Q5" s="3">
         <v>0.84</v>
       </c>
-      <c r="R5" s="9">
+      <c r="R5" s="8">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="S5" s="8">
+      <c r="S5" s="7">
         <v>0.74</v>
       </c>
       <c r="T5" s="3">
@@ -793,10 +802,10 @@
       <c r="U5" s="3">
         <v>0.74</v>
       </c>
-      <c r="V5" s="9">
+      <c r="V5" s="8">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="W5" s="8">
+      <c r="W5" s="7">
         <v>0.7</v>
       </c>
       <c r="X5" s="3">
@@ -805,18 +814,18 @@
       <c r="Y5" s="3">
         <v>0.63</v>
       </c>
-      <c r="Z5" s="9">
+      <c r="Z5" s="8">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>0.76</v>
       </c>
       <c r="D6" s="4">
@@ -828,7 +837,7 @@
       <c r="F6" s="3">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>0.73</v>
       </c>
       <c r="H6" s="3">
@@ -837,10 +846,10 @@
       <c r="I6" s="3">
         <v>0.75</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <v>0.06</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <v>0.73</v>
       </c>
       <c r="L6" s="3">
@@ -849,10 +858,10 @@
       <c r="M6" s="3">
         <v>0.8</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="8">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>0.77</v>
       </c>
       <c r="P6" s="3">
@@ -861,10 +870,10 @@
       <c r="Q6" s="3">
         <v>0.82</v>
       </c>
-      <c r="R6" s="9">
+      <c r="R6" s="8">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6" s="7">
         <v>0.72</v>
       </c>
       <c r="T6" s="3">
@@ -873,10 +882,10 @@
       <c r="U6" s="3">
         <v>0.72</v>
       </c>
-      <c r="V6" s="9">
+      <c r="V6" s="8">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="W6" s="8">
+      <c r="W6" s="7">
         <v>0.67</v>
       </c>
       <c r="X6" s="3">
@@ -885,327 +894,333 @@
       <c r="Y6" s="3">
         <v>0.62</v>
       </c>
-      <c r="Z6" s="9">
+      <c r="Z6" s="8">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>0.88</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>1.71</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>0.73</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>0.83</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>1.29</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>0.81</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>0.83</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <v>1.22</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <v>0.86</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="10">
         <v>0.88</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="11">
         <v>1.1100000000000001</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q7" s="11">
         <v>0.89</v>
       </c>
-      <c r="R7" s="13">
+      <c r="R7" s="12">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="10">
         <v>0.82</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="11">
         <v>1.3</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U7" s="11">
         <v>0.79</v>
       </c>
-      <c r="V7" s="13">
+      <c r="V7" s="12">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="W7" s="11">
+      <c r="W7" s="10">
         <v>0.79</v>
       </c>
-      <c r="X7" s="12">
+      <c r="X7" s="11">
         <v>1.54</v>
       </c>
-      <c r="Y7" s="12">
+      <c r="Y7" s="11">
         <v>0.69</v>
       </c>
-      <c r="Z7" s="13">
+      <c r="Z7" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="5" t="s">
+    <row r="8" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1.48</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.79</v>
+      </c>
+      <c r="F8" s="13">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="J8" s="13">
+        <v>6.2E-2</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.79</v>
+      </c>
+      <c r="L8" s="13">
+        <v>1.05</v>
+      </c>
+      <c r="M8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="N8" s="13">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="P8" s="13">
+        <v>0.97</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>0.93</v>
+      </c>
+      <c r="R8" s="13">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="T8" s="13">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="U8" s="13">
+        <v>0.84</v>
+      </c>
+      <c r="V8" s="13">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="W8" s="5">
+        <v>0.77</v>
+      </c>
+      <c r="X8" s="13">
+        <v>1.39</v>
+      </c>
+      <c r="Y8" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="Z8" s="13">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="AA8" s="7"/>
+    </row>
+    <row r="10" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="5" t="s">
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="5" t="s">
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="5" t="s">
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="5" t="s">
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
     </row>
-    <row r="10" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="O11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="R11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="T11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="U11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="V10" s="9" t="s">
+      <c r="V11" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.71</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1.39</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.54</v>
-      </c>
-      <c r="F11" s="9">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="G11" s="8">
-        <v>0.6</v>
-      </c>
-      <c r="H11" s="3">
-        <v>1.56</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.41</v>
-      </c>
-      <c r="J11" s="9">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="L11" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="M11" s="3">
-        <v>0.96</v>
-      </c>
-      <c r="N11" s="9">
-        <v>2E-3</v>
-      </c>
-      <c r="O11" s="8">
-        <v>0.46</v>
-      </c>
-      <c r="P11" s="3">
-        <v>0.67</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>0.89</v>
-      </c>
-      <c r="R11" s="9">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="S11" s="8">
-        <v>0.45</v>
-      </c>
-      <c r="T11" s="3">
-        <v>0.48</v>
-      </c>
-      <c r="U11" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="V11" s="9">
-        <v>8.3000000000000004E-2</v>
       </c>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.79</v>
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.71</v>
       </c>
       <c r="D12" s="3">
         <v>1.39</v>
       </c>
       <c r="E12" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="F12" s="8">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G12" s="7">
         <v>0.6</v>
-      </c>
-      <c r="F12" s="9">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0.66</v>
       </c>
       <c r="H12" s="3">
         <v>1.56</v>
       </c>
       <c r="I12" s="3">
-        <v>0.44</v>
-      </c>
-      <c r="J12" s="9">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="K12" s="8">
         <v>0.41</v>
+      </c>
+      <c r="J12" s="8">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.4</v>
       </c>
       <c r="L12" s="3">
         <v>0.45</v>
       </c>
       <c r="M12" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="N12" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="O12" s="8">
-        <v>0.5</v>
+        <v>0.96</v>
+      </c>
+      <c r="N12" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="O12" s="7">
+        <v>0.46</v>
       </c>
       <c r="P12" s="3">
         <v>0.67</v>
       </c>
       <c r="Q12" s="3">
-        <v>0.92</v>
-      </c>
-      <c r="R12" s="9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="S12" s="8">
-        <v>0.46</v>
+        <v>0.89</v>
+      </c>
+      <c r="R12" s="8">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="S12" s="7">
+        <v>0.45</v>
       </c>
       <c r="T12" s="3">
         <v>0.48</v>
@@ -1213,7 +1228,7 @@
       <c r="U12" s="3">
         <v>0.99</v>
       </c>
-      <c r="V12" s="9">
+      <c r="V12" s="8">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="W12" s="3"/>
@@ -1221,63 +1236,63 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
         <v>0</v>
       </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="10">
-        <v>0.74</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="D13" s="3">
         <v>1.39</v>
       </c>
       <c r="E13" s="3">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F13" s="9">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="G13" s="8">
-        <v>0.62</v>
+        <v>0.6</v>
+      </c>
+      <c r="F13" s="8">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0.66</v>
       </c>
       <c r="H13" s="3">
         <v>1.56</v>
       </c>
       <c r="I13" s="3">
-        <v>0.42</v>
-      </c>
-      <c r="J13" s="9">
-        <v>2.7E-2</v>
-      </c>
-      <c r="K13" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="J13" s="8">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="K13" s="7">
         <v>0.41</v>
       </c>
       <c r="L13" s="3">
         <v>0.45</v>
       </c>
       <c r="M13" s="3">
-        <v>0.96</v>
-      </c>
-      <c r="N13" s="9">
+        <v>0.98</v>
+      </c>
+      <c r="N13" s="8">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O13" s="8">
-        <v>0.46</v>
+      <c r="O13" s="7">
+        <v>0.5</v>
       </c>
       <c r="P13" s="3">
         <v>0.67</v>
       </c>
       <c r="Q13" s="3">
-        <v>0.89</v>
-      </c>
-      <c r="R13" s="9">
+        <v>0.92</v>
+      </c>
+      <c r="R13" s="8">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="S13" s="8">
-        <v>0.45</v>
+      <c r="S13" s="7">
+        <v>0.46</v>
       </c>
       <c r="T13" s="3">
         <v>0.48</v>
@@ -1285,7 +1300,7 @@
       <c r="U13" s="3">
         <v>0.99</v>
       </c>
-      <c r="V13" s="9">
+      <c r="V13" s="8">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="W13" s="3"/>
@@ -1293,92 +1308,240 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    <row r="14" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>0</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="11">
-        <v>0.83</v>
-      </c>
-      <c r="D14" s="12">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="D14" s="4">
         <v>1.39</v>
       </c>
-      <c r="E14" s="12">
-        <v>0.64</v>
-      </c>
-      <c r="F14" s="13">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="G14" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="H14" s="12">
+      <c r="E14" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F14" s="8">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0.62</v>
+      </c>
+      <c r="H14" s="3">
         <v>1.56</v>
       </c>
-      <c r="I14" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="J14" s="13">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="K14" s="11">
+      <c r="I14" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="J14" s="8">
+        <v>2.7E-2</v>
+      </c>
+      <c r="K14" s="7">
         <v>0.41</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="3">
         <v>0.45</v>
       </c>
-      <c r="M14" s="12">
-        <v>0.97</v>
-      </c>
-      <c r="N14" s="13">
+      <c r="M14" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="N14" s="8">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O14" s="11">
-        <v>0.51</v>
-      </c>
-      <c r="P14" s="12">
+      <c r="O14" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="P14" s="3">
         <v>0.67</v>
       </c>
-      <c r="Q14" s="12">
-        <v>0.91</v>
-      </c>
-      <c r="R14" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="S14" s="11">
-        <v>0.46</v>
-      </c>
-      <c r="T14" s="12">
+      <c r="Q14" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="R14" s="8">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="S14" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="T14" s="3">
         <v>0.48</v>
       </c>
-      <c r="U14" s="12">
+      <c r="U14" s="3">
         <v>0.99</v>
       </c>
-      <c r="V14" s="13">
-        <v>8.2000000000000003E-2</v>
+      <c r="V14" s="8">
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
+    <row r="15" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1.39</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="F15" s="12">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.74</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1.56</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="12">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0.41</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="M15" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="N15" s="12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O15" s="10">
+        <v>0.51</v>
+      </c>
+      <c r="P15" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>0.91</v>
+      </c>
+      <c r="R15" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="S15" s="10">
+        <v>0.46</v>
+      </c>
+      <c r="T15" s="11">
+        <v>0.48</v>
+      </c>
+      <c r="U15" s="11">
+        <v>0.99</v>
+      </c>
+      <c r="V15" s="12">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+    </row>
+    <row r="16" spans="1:27" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.74</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="J16" s="6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="N16" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="P16" s="1">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="R16" s="1">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="S16" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="T16" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="V16" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="11:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="S9:V9"/>
-    <mergeCell ref="W9:Z9"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="W10:Z10"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
     <mergeCell ref="W2:Z2"/>
-    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="S10:V10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>